<commit_message>
Nuevo set de datos con 96 columnas sin errores
</commit_message>
<xml_diff>
--- a/set_datos.xlsx
+++ b/set_datos.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santinobanana\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9845BD-0798-4051-B6B6-1D0A1FC31EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB8822C-19EF-4757-A56D-17DBFC81FEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{697A5128-6904-46DA-BF5F-8901020213D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{697A5128-6904-46DA-BF5F-8901020213D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="131">
   <si>
     <t>C1</t>
   </si>
@@ -88,30 +91,6 @@
     <t>C15</t>
   </si>
   <si>
-    <t>20.6546856 -103.3599066</t>
-  </si>
-  <si>
-    <t>20.6856283 -103.3603916</t>
-  </si>
-  <si>
-    <t>20.6037028 -103.2340488</t>
-  </si>
-  <si>
-    <t>21.3707639 -101.9781741</t>
-  </si>
-  <si>
-    <t>22.7757058 -102.5549564</t>
-  </si>
-  <si>
-    <t>26.7549602 -100.1159915</t>
-  </si>
-  <si>
-    <t>25.2144143 -111.6296634</t>
-  </si>
-  <si>
-    <t>15.8446086 -89.8489378</t>
-  </si>
-  <si>
     <t>C16</t>
   </si>
   <si>
@@ -322,9 +301,6 @@
     <t>23.8546621, -108.6009987</t>
   </si>
   <si>
-    <t>22.1098692, -114.3218962</t>
-  </si>
-  <si>
     <t>31.5102666, -109.8614469</t>
   </si>
   <si>
@@ -389,6 +365,75 @@
   </si>
   <si>
     <t>C43</t>
+  </si>
+  <si>
+    <t>-34.567, -56.789</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12.345, 67.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -23.456, 45.678</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.123, -12.345</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89.012, -34.567</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -56.789, 12.345</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67.890, -23.456</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -45.678, 0.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12.345, 89.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -34.567, -56.789</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45.678, 67.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -12.345, -23.456</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.123, 89.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -56.789, -34.567</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67.890, 12.345</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89.012, 0.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -34.567, 67.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12.345, -23.456</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -56.789, 45.678</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.123, -34.567</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67.890, 89.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -23.456, 12.345</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45.678, 0.123</t>
   </si>
 </sst>
 </file>
@@ -745,14 +790,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DFC37B-7156-4323-8050-945060E21D99}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -779,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -790,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -801,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -812,7 +857,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>35</v>
@@ -823,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>-20</v>
@@ -834,7 +879,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>0.8</v>
@@ -845,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -856,7 +901,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -867,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -875,6 +920,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -882,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE638EC7-9B47-4EF4-A75D-9FE995007683}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +942,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -915,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -926,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -937,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -948,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -959,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>35</v>
@@ -970,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>-20</v>
@@ -981,7 +1027,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>0.8</v>
@@ -992,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -1003,7 +1049,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -1014,7 +1060,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1025,7 +1071,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1036,7 +1082,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1047,7 +1093,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1058,7 +1104,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -1066,10 +1112,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -1077,10 +1123,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1088,10 +1134,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -1099,10 +1145,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1110,10 +1156,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1121,10 +1167,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1132,10 +1178,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1143,10 +1189,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1154,10 +1200,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1165,10 +1211,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1176,10 +1222,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -1187,10 +1233,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -1198,10 +1244,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1209,10 +1255,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1220,10 +1266,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1231,10 +1277,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1242,10 +1288,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1253,10 +1299,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1264,10 +1310,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1275,10 +1321,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1286,10 +1332,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1297,10 +1343,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -1308,10 +1354,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -1319,10 +1365,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -1330,10 +1376,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C41">
         <v>7</v>
@@ -1341,10 +1387,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>3</v>
@@ -1352,10 +1398,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C43">
         <v>8</v>
@@ -1363,10 +1409,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C44">
         <v>9</v>
@@ -1382,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D3951E-1CBE-4C53-A815-A9CE4A6181A5}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C14" sqref="C12:C14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1442,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1415,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1426,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1437,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1448,7 +1494,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1459,7 +1505,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1470,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1481,7 +1527,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1492,7 +1538,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1503,7 +1549,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C11">
         <v>125</v>
@@ -1514,7 +1560,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C12">
         <v>35</v>
@@ -1525,7 +1571,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C13">
         <v>-20</v>
@@ -1536,7 +1582,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C14">
         <v>0.8</v>
@@ -1547,7 +1593,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1558,7 +1604,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -1566,10 +1612,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1577,10 +1623,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -1588,10 +1634,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1599,10 +1645,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -1610,10 +1656,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -1621,10 +1667,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1632,10 +1678,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1643,13 +1689,1716 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9680D481-6E8B-4A87-B6E2-6B298D2CD960}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7686F78E-5E8E-4698-98CC-2E3FDB03B85E}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84935178-B8B6-4C1B-A260-DC6C49CD2501}">
+  <dimension ref="A1:C96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f t="shared" ref="A2:A65" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>115</v>
       </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
       <c r="C24">
-        <v>3</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" ref="A66:A96" si="1">ROW(A66)</f>
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>130</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>122</v>
+      </c>
+      <c r="C87">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>123</v>
+      </c>
+      <c r="C89">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>124</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>125</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>126</v>
+      </c>
+      <c r="C92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>127</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>130</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>